<commit_message>
update_10.03.2019 - changed cellstyle methods
</commit_message>
<xml_diff>
--- a/src/main/resources/calculation.xlsx
+++ b/src/main/resources/calculation.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист0" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -55,10 +55,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -339,7 +337,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="L1:O4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -352,34 +350,9 @@
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" customWidth="1"/>
-    <col min="12" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="12" max="15" width="12.85546875" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>